<commit_message>
final code with mat model
</commit_message>
<xml_diff>
--- a/Objective values.xlsx
+++ b/Objective values.xlsx
@@ -402,10 +402,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2821</v>
+        <v>498</v>
       </c>
       <c r="C2">
-        <v>850</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -413,10 +413,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2772</v>
+        <v>508</v>
       </c>
       <c r="C3">
-        <v>837</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -424,10 +424,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2799</v>
+        <v>472</v>
       </c>
       <c r="C4">
-        <v>847</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -435,10 +435,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2772</v>
+        <v>420</v>
       </c>
       <c r="C5">
-        <v>837</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -446,10 +446,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2787</v>
+        <v>518</v>
       </c>
       <c r="C6">
-        <v>982</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -457,10 +457,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2772</v>
+        <v>507</v>
       </c>
       <c r="C7">
-        <v>837</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -468,10 +468,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2772</v>
+        <v>419</v>
       </c>
       <c r="C8">
-        <v>837</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -479,10 +479,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2865</v>
+        <v>466</v>
       </c>
       <c r="C9">
-        <v>867</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -490,10 +490,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2772</v>
+        <v>407</v>
       </c>
       <c r="C10">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -501,10 +501,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2869</v>
+        <v>407</v>
       </c>
       <c r="C11">
-        <v>866</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -512,10 +512,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>2779</v>
+        <v>528</v>
       </c>
       <c r="C12">
-        <v>857</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -523,10 +523,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2764</v>
+        <v>466</v>
       </c>
       <c r="C13">
-        <v>837</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -534,10 +534,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2744</v>
+        <v>507</v>
       </c>
       <c r="C14">
-        <v>837</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -545,10 +545,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2763</v>
+        <v>407</v>
       </c>
       <c r="C15">
-        <v>943</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -556,10 +556,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>2815</v>
+        <v>407</v>
       </c>
       <c r="C16">
-        <v>858</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -567,10 +567,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>2787</v>
+        <v>407</v>
       </c>
       <c r="C17">
-        <v>846</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -578,10 +578,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2744</v>
+        <v>466</v>
       </c>
       <c r="C18">
-        <v>837</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -589,10 +589,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2849</v>
+        <v>407</v>
       </c>
       <c r="C19">
-        <v>847</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -600,10 +600,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>2920</v>
+        <v>419</v>
       </c>
       <c r="C20">
-        <v>867</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -611,10 +611,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>2750</v>
+        <v>407</v>
       </c>
       <c r="C21">
-        <v>857</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -622,10 +622,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2744</v>
+        <v>407</v>
       </c>
       <c r="C22">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -633,10 +633,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2741</v>
+        <v>407</v>
       </c>
       <c r="C23">
-        <v>845</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -644,10 +644,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2859</v>
+        <v>442</v>
       </c>
       <c r="C24">
-        <v>867</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -655,10 +655,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2683</v>
+        <v>407</v>
       </c>
       <c r="C25">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -666,10 +666,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2775</v>
+        <v>457</v>
       </c>
       <c r="C26">
-        <v>876</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -677,10 +677,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2781</v>
+        <v>407</v>
       </c>
       <c r="C27">
-        <v>855</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -688,10 +688,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2683</v>
+        <v>407</v>
       </c>
       <c r="C28">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -699,10 +699,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>2720</v>
+        <v>518</v>
       </c>
       <c r="C29">
-        <v>876</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -710,10 +710,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2683</v>
+        <v>407</v>
       </c>
       <c r="C30">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -721,10 +721,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>2768</v>
+        <v>517</v>
       </c>
       <c r="C31">
-        <v>886</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -732,10 +732,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>2690</v>
+        <v>431</v>
       </c>
       <c r="C32">
-        <v>929</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -743,10 +743,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>2777</v>
+        <v>435</v>
       </c>
       <c r="C33">
-        <v>877</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -754,10 +754,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>2614</v>
+        <v>507</v>
       </c>
       <c r="C34">
-        <v>837</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -765,10 +765,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>2712</v>
+        <v>458</v>
       </c>
       <c r="C35">
-        <v>847</v>
+        <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -776,10 +776,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>2610</v>
+        <v>407</v>
       </c>
       <c r="C36">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -787,10 +787,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>2620</v>
+        <v>431</v>
       </c>
       <c r="C37">
-        <v>899</v>
+        <v>290</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -798,10 +798,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>2611</v>
+        <v>436</v>
       </c>
       <c r="C38">
-        <v>838</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -809,10 +809,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>2707</v>
+        <v>498</v>
       </c>
       <c r="C39">
-        <v>867</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -820,10 +820,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>2610</v>
+        <v>407</v>
       </c>
       <c r="C40">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -831,10 +831,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>2689</v>
+        <v>407</v>
       </c>
       <c r="C41">
-        <v>846</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -842,10 +842,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>2610</v>
+        <v>407</v>
       </c>
       <c r="C42">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -853,10 +853,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>2697</v>
+        <v>402</v>
       </c>
       <c r="C43">
-        <v>864</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -864,10 +864,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>2592</v>
+        <v>523</v>
       </c>
       <c r="C44">
-        <v>911</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -875,10 +875,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>2559</v>
+        <v>402</v>
       </c>
       <c r="C45">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -886,10 +886,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>2606</v>
+        <v>402</v>
       </c>
       <c r="C46">
-        <v>869</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -897,10 +897,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>2585</v>
+        <v>402</v>
       </c>
       <c r="C47">
-        <v>853</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -908,10 +908,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>2559</v>
+        <v>493</v>
       </c>
       <c r="C48">
-        <v>837</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -919,10 +919,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>2683</v>
+        <v>503</v>
       </c>
       <c r="C49">
-        <v>863</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -930,10 +930,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>2640</v>
+        <v>435</v>
       </c>
       <c r="C50">
-        <v>847</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -941,10 +941,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>2559</v>
+        <v>402</v>
       </c>
       <c r="C51">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -952,10 +952,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>2559</v>
+        <v>494</v>
       </c>
       <c r="C52">
-        <v>837</v>
+        <v>290</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -963,10 +963,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>2581</v>
+        <v>412</v>
       </c>
       <c r="C53">
-        <v>856</v>
+        <v>289</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -974,10 +974,10 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>2556</v>
+        <v>448</v>
       </c>
       <c r="C54">
-        <v>837</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -985,10 +985,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>2560</v>
+        <v>431</v>
       </c>
       <c r="C55">
-        <v>842</v>
+        <v>280</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -996,10 +996,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>2619</v>
+        <v>402</v>
       </c>
       <c r="C56">
-        <v>858</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1007,10 +1007,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>2556</v>
+        <v>402</v>
       </c>
       <c r="C57">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1018,10 +1018,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>2581</v>
+        <v>401</v>
       </c>
       <c r="C58">
-        <v>856</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1029,10 +1029,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>2610</v>
+        <v>402</v>
       </c>
       <c r="C59">
-        <v>856</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1040,10 +1040,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>2556</v>
+        <v>502</v>
       </c>
       <c r="C60">
-        <v>837</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1051,10 +1051,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>2658</v>
+        <v>447</v>
       </c>
       <c r="C61">
-        <v>876</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1062,10 +1062,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>2681</v>
+        <v>402</v>
       </c>
       <c r="C62">
-        <v>955</v>
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1073,10 +1073,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>2590</v>
+        <v>401</v>
       </c>
       <c r="C63">
-        <v>901</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1084,10 +1084,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>2580</v>
+        <v>402</v>
       </c>
       <c r="C64">
-        <v>901</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1095,10 +1095,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>2716</v>
+        <v>495</v>
       </c>
       <c r="C65">
-        <v>852</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1106,10 +1106,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>2567</v>
+        <v>503</v>
       </c>
       <c r="C66">
-        <v>973</v>
+        <v>280</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1117,10 +1117,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>2553</v>
+        <v>402</v>
       </c>
       <c r="C67">
-        <v>853</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1128,10 +1128,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>2627</v>
+        <v>503</v>
       </c>
       <c r="C68">
-        <v>934</v>
+        <v>280</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1139,10 +1139,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>2567</v>
+        <v>431</v>
       </c>
       <c r="C69">
-        <v>926</v>
+        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1150,10 +1150,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>2636</v>
+        <v>402</v>
       </c>
       <c r="C70">
-        <v>857</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1161,10 +1161,10 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>2658</v>
+        <v>402</v>
       </c>
       <c r="C71">
-        <v>943</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1172,10 +1172,10 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>2553</v>
+        <v>447</v>
       </c>
       <c r="C72">
-        <v>837</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1183,10 +1183,10 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>2553</v>
+        <v>402</v>
       </c>
       <c r="C73">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1194,10 +1194,10 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>2636</v>
+        <v>523</v>
       </c>
       <c r="C74">
-        <v>904</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1205,10 +1205,10 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>2637</v>
+        <v>447</v>
       </c>
       <c r="C75">
-        <v>867</v>
+        <v>289</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1216,10 +1216,10 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>2553</v>
+        <v>451</v>
       </c>
       <c r="C76">
-        <v>837</v>
+        <v>250</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1227,10 +1227,10 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>2553</v>
+        <v>402</v>
       </c>
       <c r="C77">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1238,10 +1238,10 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>2660</v>
+        <v>402</v>
       </c>
       <c r="C78">
-        <v>901</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1249,10 +1249,10 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>2620</v>
+        <v>523</v>
       </c>
       <c r="C79">
-        <v>847</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1260,10 +1260,10 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>2540</v>
+        <v>402</v>
       </c>
       <c r="C80">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1271,10 +1271,10 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>2587</v>
+        <v>402</v>
       </c>
       <c r="C81">
-        <v>857</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1282,10 +1282,10 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>2645</v>
+        <v>402</v>
       </c>
       <c r="C82">
-        <v>868</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1293,10 +1293,10 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>2622</v>
+        <v>451</v>
       </c>
       <c r="C83">
-        <v>857</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1304,10 +1304,10 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>2685</v>
+        <v>402</v>
       </c>
       <c r="C84">
-        <v>865</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1315,10 +1315,10 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>2606</v>
+        <v>432</v>
       </c>
       <c r="C85">
-        <v>857</v>
+        <v>289</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1326,10 +1326,10 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>2555</v>
+        <v>402</v>
       </c>
       <c r="C86">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1337,10 +1337,10 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>2553</v>
+        <v>412</v>
       </c>
       <c r="C87">
-        <v>888</v>
+        <v>289</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1348,10 +1348,10 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>2715</v>
+        <v>405</v>
       </c>
       <c r="C88">
-        <v>881</v>
+        <v>289</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1359,10 +1359,10 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>2640</v>
+        <v>451</v>
       </c>
       <c r="C89">
-        <v>914</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1370,10 +1370,10 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>2589</v>
+        <v>401</v>
       </c>
       <c r="C90">
-        <v>861</v>
+        <v>189</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1381,10 +1381,10 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>2617</v>
+        <v>402</v>
       </c>
       <c r="C91">
-        <v>845</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1392,10 +1392,10 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>2624</v>
+        <v>402</v>
       </c>
       <c r="C92">
-        <v>916</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1403,10 +1403,10 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>2595</v>
+        <v>461</v>
       </c>
       <c r="C93">
-        <v>844</v>
+        <v>279</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1414,10 +1414,10 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>2540</v>
+        <v>402</v>
       </c>
       <c r="C94">
-        <v>837</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1425,10 +1425,10 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>2548</v>
+        <v>496</v>
       </c>
       <c r="C95">
-        <v>914</v>
+        <v>210</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1436,10 +1436,10 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>2683</v>
+        <v>402</v>
       </c>
       <c r="C96">
-        <v>868</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1447,10 +1447,10 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>2544</v>
+        <v>467</v>
       </c>
       <c r="C97">
-        <v>942</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1458,10 +1458,10 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>2541</v>
+        <v>402</v>
       </c>
       <c r="C98">
-        <v>838</v>
+        <v>190</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1469,10 +1469,10 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>2619</v>
+        <v>402</v>
       </c>
       <c r="C99">
-        <v>900</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1480,10 +1480,10 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>2588</v>
+        <v>503</v>
       </c>
       <c r="C100">
-        <v>860</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1491,10 +1491,10 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>2715</v>
+        <v>402</v>
       </c>
       <c r="C101">
-        <v>881</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
math and heuristic difff
</commit_message>
<xml_diff>
--- a/Objective values.xlsx
+++ b/Objective values.xlsx
@@ -402,10 +402,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>498</v>
+        <v>142</v>
       </c>
       <c r="C2">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -413,10 +413,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>508</v>
+        <v>142</v>
       </c>
       <c r="C3">
-        <v>280</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -424,10 +424,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>472</v>
+        <v>172</v>
       </c>
       <c r="C4">
-        <v>210</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -435,10 +435,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>420</v>
+        <v>145</v>
       </c>
       <c r="C5">
-        <v>290</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -446,10 +446,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>518</v>
+        <v>142</v>
       </c>
       <c r="C6">
-        <v>230</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -457,10 +457,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>507</v>
+        <v>142</v>
       </c>
       <c r="C7">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -468,10 +468,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>419</v>
+        <v>140</v>
       </c>
       <c r="C8">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -479,10 +479,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>466</v>
+        <v>143</v>
       </c>
       <c r="C9">
-        <v>279</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -490,10 +490,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C10">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -501,10 +501,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>407</v>
+        <v>167</v>
       </c>
       <c r="C11">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -512,10 +512,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>528</v>
+        <v>167</v>
       </c>
       <c r="C12">
-        <v>220</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -523,10 +523,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>466</v>
+        <v>140</v>
       </c>
       <c r="C13">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -534,10 +534,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>507</v>
+        <v>140</v>
       </c>
       <c r="C14">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -545,10 +545,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C15">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -556,10 +556,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>407</v>
+        <v>151</v>
       </c>
       <c r="C16">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -567,10 +567,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C17">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -578,10 +578,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>466</v>
+        <v>140</v>
       </c>
       <c r="C18">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -589,10 +589,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C19">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -600,10 +600,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>419</v>
+        <v>143</v>
       </c>
       <c r="C20">
-        <v>289</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -611,10 +611,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C21">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -622,10 +622,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>407</v>
+        <v>147</v>
       </c>
       <c r="C22">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -633,10 +633,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C23">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -644,10 +644,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>442</v>
+        <v>140</v>
       </c>
       <c r="C24">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -655,10 +655,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C25">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -666,10 +666,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>457</v>
+        <v>140</v>
       </c>
       <c r="C26">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -677,10 +677,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C27">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -688,10 +688,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>407</v>
+        <v>147</v>
       </c>
       <c r="C28">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -699,10 +699,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>518</v>
+        <v>140</v>
       </c>
       <c r="C29">
-        <v>230</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -710,10 +710,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>407</v>
+        <v>151</v>
       </c>
       <c r="C30">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -721,10 +721,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>517</v>
+        <v>140</v>
       </c>
       <c r="C31">
-        <v>229</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -732,10 +732,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>431</v>
+        <v>166</v>
       </c>
       <c r="C32">
-        <v>290</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -743,10 +743,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>435</v>
+        <v>166</v>
       </c>
       <c r="C33">
-        <v>279</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -754,10 +754,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>507</v>
+        <v>140</v>
       </c>
       <c r="C34">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -765,10 +765,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>458</v>
+        <v>143</v>
       </c>
       <c r="C35">
-        <v>290</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -776,10 +776,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>407</v>
+        <v>167</v>
       </c>
       <c r="C36">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -787,10 +787,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>431</v>
+        <v>166</v>
       </c>
       <c r="C37">
-        <v>290</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -798,10 +798,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>436</v>
+        <v>166</v>
       </c>
       <c r="C38">
-        <v>280</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -809,10 +809,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>498</v>
+        <v>170</v>
       </c>
       <c r="C39">
-        <v>289</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -820,10 +820,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>407</v>
+        <v>140</v>
       </c>
       <c r="C40">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -831,10 +831,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>407</v>
+        <v>167</v>
       </c>
       <c r="C41">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -842,10 +842,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>407</v>
+        <v>167</v>
       </c>
       <c r="C42">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -853,10 +853,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>402</v>
+        <v>150</v>
       </c>
       <c r="C43">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -864,10 +864,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>523</v>
+        <v>140</v>
       </c>
       <c r="C44">
-        <v>220</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -875,10 +875,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C45">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -886,10 +886,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C46">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -897,10 +897,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C47">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -908,10 +908,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>493</v>
+        <v>161</v>
       </c>
       <c r="C48">
-        <v>289</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -919,10 +919,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>503</v>
+        <v>140</v>
       </c>
       <c r="C49">
-        <v>280</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -930,10 +930,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>435</v>
+        <v>140</v>
       </c>
       <c r="C50">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -941,10 +941,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C51">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -952,10 +952,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>494</v>
+        <v>140</v>
       </c>
       <c r="C52">
-        <v>290</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -963,10 +963,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>412</v>
+        <v>148</v>
       </c>
       <c r="C53">
-        <v>289</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -974,10 +974,10 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>448</v>
+        <v>140</v>
       </c>
       <c r="C54">
-        <v>290</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -985,10 +985,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>431</v>
+        <v>140</v>
       </c>
       <c r="C55">
-        <v>280</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -996,10 +996,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C56">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1007,10 +1007,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C57">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1018,10 +1018,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>401</v>
+        <v>140</v>
       </c>
       <c r="C58">
-        <v>189</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1029,10 +1029,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>402</v>
+        <v>148</v>
       </c>
       <c r="C59">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1040,10 +1040,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>502</v>
+        <v>140</v>
       </c>
       <c r="C60">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1051,10 +1051,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>447</v>
+        <v>167</v>
       </c>
       <c r="C61">
-        <v>289</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1062,10 +1062,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C62">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1073,10 +1073,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>401</v>
+        <v>151</v>
       </c>
       <c r="C63">
-        <v>189</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1084,10 +1084,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>402</v>
+        <v>167</v>
       </c>
       <c r="C64">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1095,10 +1095,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>495</v>
+        <v>140</v>
       </c>
       <c r="C65">
-        <v>209</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1106,10 +1106,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>503</v>
+        <v>150</v>
       </c>
       <c r="C66">
-        <v>280</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1117,10 +1117,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C67">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1128,10 +1128,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>503</v>
+        <v>140</v>
       </c>
       <c r="C68">
-        <v>280</v>
+        <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1139,10 +1139,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>431</v>
+        <v>140</v>
       </c>
       <c r="C69">
-        <v>280</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1150,10 +1150,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>402</v>
+        <v>150</v>
       </c>
       <c r="C70">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1161,10 +1161,10 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>402</v>
+        <v>167</v>
       </c>
       <c r="C71">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1172,10 +1172,10 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>447</v>
+        <v>140</v>
       </c>
       <c r="C72">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1183,10 +1183,10 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>402</v>
+        <v>144</v>
       </c>
       <c r="C73">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1194,10 +1194,10 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>523</v>
+        <v>140</v>
       </c>
       <c r="C74">
-        <v>220</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1205,10 +1205,10 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>447</v>
+        <v>140</v>
       </c>
       <c r="C75">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1216,10 +1216,10 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>451</v>
+        <v>166</v>
       </c>
       <c r="C76">
-        <v>250</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1227,10 +1227,10 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C77">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1238,10 +1238,10 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C78">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1249,10 +1249,10 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>523</v>
+        <v>140</v>
       </c>
       <c r="C79">
-        <v>220</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1260,10 +1260,10 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C80">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1271,10 +1271,10 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>402</v>
+        <v>144</v>
       </c>
       <c r="C81">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1282,10 +1282,10 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>402</v>
+        <v>150</v>
       </c>
       <c r="C82">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1293,10 +1293,10 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>451</v>
+        <v>150</v>
       </c>
       <c r="C83">
-        <v>250</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1304,10 +1304,10 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>402</v>
+        <v>150</v>
       </c>
       <c r="C84">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1315,10 +1315,10 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>432</v>
+        <v>167</v>
       </c>
       <c r="C85">
-        <v>289</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1326,10 +1326,10 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C86">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1337,10 +1337,10 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>412</v>
+        <v>140</v>
       </c>
       <c r="C87">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1348,10 +1348,10 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>405</v>
+        <v>140</v>
       </c>
       <c r="C88">
-        <v>289</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1359,10 +1359,10 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>451</v>
+        <v>144</v>
       </c>
       <c r="C89">
-        <v>250</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1370,10 +1370,10 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>401</v>
+        <v>140</v>
       </c>
       <c r="C90">
-        <v>189</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1381,10 +1381,10 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>402</v>
+        <v>143</v>
       </c>
       <c r="C91">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1392,10 +1392,10 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C92">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1403,10 +1403,10 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>461</v>
+        <v>143</v>
       </c>
       <c r="C93">
-        <v>279</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1414,10 +1414,10 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>402</v>
+        <v>161</v>
       </c>
       <c r="C94">
-        <v>190</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1425,10 +1425,10 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>496</v>
+        <v>140</v>
       </c>
       <c r="C95">
-        <v>210</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1436,10 +1436,10 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>402</v>
+        <v>139</v>
       </c>
       <c r="C96">
-        <v>190</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1447,10 +1447,10 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>467</v>
+        <v>140</v>
       </c>
       <c r="C97">
-        <v>210</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1458,10 +1458,10 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C98">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1469,10 +1469,10 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>402</v>
+        <v>148</v>
       </c>
       <c r="C99">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1480,10 +1480,10 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>503</v>
+        <v>167</v>
       </c>
       <c r="C100">
-        <v>280</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1491,10 +1491,10 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>402</v>
+        <v>140</v>
       </c>
       <c r="C101">
-        <v>190</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>